<commit_message>
updated data and added new merge and clean notebook
</commit_message>
<xml_diff>
--- a/AnatomyPoints.xlsx
+++ b/AnatomyPoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\S-Files\LDW Strategy\Users\David Ly\Projects\Corona\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Ly\Documents\Programming\COVID19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B82DB3F-F16A-4D2F-BB2F-CA90C9EBE939}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3609E34-A0C1-413E-93D4-071465DA6150}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58260" yWindow="3450" windowWidth="15150" windowHeight="12195" xr2:uid="{EDC8D9BE-FCD9-442A-9275-C5CC5980A80B}"/>
+    <workbookView xWindow="-44160" yWindow="2070" windowWidth="22590" windowHeight="14745" xr2:uid="{EDC8D9BE-FCD9-442A-9275-C5CC5980A80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Position</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Gastrointestinal Issues</t>
+  </si>
+  <si>
+    <t>Loss of Smell or Taste</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B0EF46-D85D-453E-AF0B-3A929C82BE83}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +466,7 @@
         <v>7.5</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,13 +474,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.5999999999999996</v>
+        <v>4.5</v>
       </c>
       <c r="C4">
-        <v>6.2</v>
+        <v>7.5</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -485,12 +488,26 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C5">
+        <v>6.2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2.7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>